<commit_message>
parent 501a1933986ea44ca9cc72fd0a1498b1c436b361 author Adam Shimali <adam.shimali@gmail.com> 1757947303 +0100 committer Adam Shimali <adam.shimali@gmail.com> 1758188002 +0100
tool: JSON Schema generation script added. Uses similar approach to
spreadsheet generation. Traverses specification and outputs JSON schema
(Draft-07) for each individual planning application type.

See docs/json-schema-generation.md for details of approach and
implementation

add json schema generation doc
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/development-relating-to-the-onshore-extraction-of-oil-and-gas-extraction-oil-gas.xlsx
+++ b/generated/spreadsheet/development-relating-to-the-onshore-extraction-of-oil-and-gas-extraction-oil-gas.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I162"/>
+  <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5171,28 +5171,36 @@
           <t>Details of trees and/or hedges that will be affected by the proposed development</t>
         </is>
       </c>
-      <c r="C151" s="2" t="inlineStr"/>
+      <c r="C151" s="2" t="inlineStr">
+        <is>
+          <t>Trees on site</t>
+        </is>
+      </c>
       <c r="D151" s="2" t="inlineStr"/>
       <c r="E151" s="2" t="inlineStr"/>
       <c r="F151" s="2" t="inlineStr"/>
-      <c r="G151" s="2" t="inlineStr"/>
-      <c r="H151" s="2" t="inlineStr"/>
-      <c r="I151" s="2" t="inlineStr"/>
+      <c r="G151" s="2" t="inlineStr">
+        <is>
+          <t>Whether trees or hedges are present on the proposed development site</t>
+        </is>
+      </c>
+      <c r="H151" s="2" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="I151" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
     </row>
     <row r="152">
-      <c r="A152" s="2" t="inlineStr">
-        <is>
-          <t>Development type</t>
-        </is>
-      </c>
-      <c r="B152" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Supporting information for developments used for oil and gas exploration or mining </t>
-        </is>
-      </c>
+      <c r="A152" s="2" t="n"/>
+      <c r="B152" s="2" t="n"/>
       <c r="C152" s="2" t="inlineStr">
         <is>
-          <t>Development phase</t>
+          <t>Trees on adjacent land</t>
         </is>
       </c>
       <c r="D152" s="2" t="inlineStr"/>
@@ -5200,12 +5208,12 @@
       <c r="F152" s="2" t="inlineStr"/>
       <c r="G152" s="2" t="inlineStr">
         <is>
-          <t>Phases of oil and gas development the application covers</t>
+          <t>Whether trees or hedges on land adjacent to the proposed development site could influence the development or might be important as part of the local landscape character</t>
         </is>
       </c>
       <c r="H152" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I152" s="2" t="inlineStr">
@@ -5215,11 +5223,19 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="2" t="n"/>
-      <c r="B153" s="2" t="n"/>
+      <c r="A153" s="2" t="inlineStr">
+        <is>
+          <t>Development type</t>
+        </is>
+      </c>
+      <c r="B153" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Supporting information for developments used for oil and gas exploration or mining </t>
+        </is>
+      </c>
       <c r="C153" s="2" t="inlineStr">
         <is>
-          <t>Development description</t>
+          <t>Development phase</t>
         </is>
       </c>
       <c r="D153" s="2" t="inlineStr"/>
@@ -5227,12 +5243,12 @@
       <c r="F153" s="2" t="inlineStr"/>
       <c r="G153" s="2" t="inlineStr">
         <is>
-          <t>Brief description of the development, including main oils, gases, and machinery</t>
+          <t>Phases of oil and gas development the application covers</t>
         </is>
       </c>
       <c r="H153" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I153" s="2" t="inlineStr">
@@ -5246,7 +5262,7 @@
       <c r="B154" s="2" t="n"/>
       <c r="C154" s="2" t="inlineStr">
         <is>
-          <t>Quantity cubic metres</t>
+          <t>Development description</t>
         </is>
       </c>
       <c r="D154" s="2" t="inlineStr"/>
@@ -5254,12 +5270,12 @@
       <c r="F154" s="2" t="inlineStr"/>
       <c r="G154" s="2" t="inlineStr">
         <is>
-          <t>Quantity of oil or gas involved in cubic metres</t>
+          <t>Brief description of the development, including main oils, gases, and machinery</t>
         </is>
       </c>
       <c r="H154" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I154" s="2" t="inlineStr">
@@ -5273,7 +5289,7 @@
       <c r="B155" s="2" t="n"/>
       <c r="C155" s="2" t="inlineStr">
         <is>
-          <t>Permission period years</t>
+          <t>Quantity cubic metres</t>
         </is>
       </c>
       <c r="D155" s="2" t="inlineStr"/>
@@ -5281,7 +5297,7 @@
       <c r="F155" s="2" t="inlineStr"/>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Period of permission sought in years</t>
+          <t>Quantity of oil or gas involved in cubic metres</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -5291,7 +5307,7 @@
       </c>
       <c r="I155" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -5300,7 +5316,7 @@
       <c r="B156" s="2" t="n"/>
       <c r="C156" s="2" t="inlineStr">
         <is>
-          <t>Hydrocarbon licence block</t>
+          <t>Permission period years</t>
         </is>
       </c>
       <c r="D156" s="2" t="inlineStr"/>
@@ -5308,17 +5324,17 @@
       <c r="F156" s="2" t="inlineStr"/>
       <c r="G156" s="2" t="inlineStr">
         <is>
-          <t>Hydrocarbon licence block where the development is located</t>
+          <t>Period of permission sought in years</t>
         </is>
       </c>
       <c r="H156" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I156" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -5327,7 +5343,7 @@
       <c r="B157" s="2" t="n"/>
       <c r="C157" s="2" t="inlineStr">
         <is>
-          <t>Surface site area hectares</t>
+          <t>Hydrocarbon licence block</t>
         </is>
       </c>
       <c r="D157" s="2" t="inlineStr"/>
@@ -5335,17 +5351,17 @@
       <c r="F157" s="2" t="inlineStr"/>
       <c r="G157" s="2" t="inlineStr">
         <is>
-          <t>Surface site area in hectares</t>
+          <t>Hydrocarbon licence block where the development is located</t>
         </is>
       </c>
       <c r="H157" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I157" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -5354,7 +5370,7 @@
       <c r="B158" s="2" t="n"/>
       <c r="C158" s="2" t="inlineStr">
         <is>
-          <t>Site hectares provided by</t>
+          <t>Surface site area hectares</t>
         </is>
       </c>
       <c r="D158" s="2" t="inlineStr"/>
@@ -5362,12 +5378,12 @@
       <c r="F158" s="2" t="inlineStr"/>
       <c r="G158" s="2" t="inlineStr">
         <is>
-          <t>Who provided the site hectares value (applicant or system)</t>
+          <t>Surface site area in hectares</t>
         </is>
       </c>
       <c r="H158" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I158" s="2" t="inlineStr">
@@ -5381,7 +5397,7 @@
       <c r="B159" s="2" t="n"/>
       <c r="C159" s="2" t="inlineStr">
         <is>
-          <t>Environmental statement</t>
+          <t>Site hectares provided by</t>
         </is>
       </c>
       <c r="D159" s="2" t="inlineStr"/>
@@ -5389,17 +5405,17 @@
       <c r="F159" s="2" t="inlineStr"/>
       <c r="G159" s="2" t="inlineStr">
         <is>
-          <t>Is an Environmental Statement attached to the application</t>
+          <t>Who provided the site hectares value (applicant or system)</t>
         </is>
       </c>
       <c r="H159" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I159" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -5408,7 +5424,7 @@
       <c r="B160" s="2" t="n"/>
       <c r="C160" s="2" t="inlineStr">
         <is>
-          <t>Environmental statement reference</t>
+          <t>Environmental statement</t>
         </is>
       </c>
       <c r="D160" s="2" t="inlineStr"/>
@@ -5416,34 +5432,26 @@
       <c r="F160" s="2" t="inlineStr"/>
       <c r="G160" s="2" t="inlineStr">
         <is>
-          <t>Reference to the environmental statement document</t>
+          <t>Is an Environmental Statement attached to the application</t>
         </is>
       </c>
       <c r="H160" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I160" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="2" t="inlineStr">
-        <is>
-          <t>Voluntary agreement</t>
-        </is>
-      </c>
-      <c r="B161" s="2" t="inlineStr">
-        <is>
-          <t>Details of any voluntary agreements made as part of an oil and gas extraction application.</t>
-        </is>
-      </c>
+      <c r="A161" s="2" t="n"/>
+      <c r="B161" s="2" t="n"/>
       <c r="C161" s="2" t="inlineStr">
         <is>
-          <t>Draft agreement included</t>
+          <t>Environmental statement reference</t>
         </is>
       </c>
       <c r="D161" s="2" t="inlineStr"/>
@@ -5451,26 +5459,34 @@
       <c r="F161" s="2" t="inlineStr"/>
       <c r="G161" s="2" t="inlineStr">
         <is>
-          <t>Has an outline or draft agreement been included? (True / False)</t>
+          <t>Reference to the environmental statement document</t>
         </is>
       </c>
       <c r="H161" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I161" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="2" t="n"/>
-      <c r="B162" s="2" t="n"/>
+      <c r="A162" s="2" t="inlineStr">
+        <is>
+          <t>Voluntary agreement</t>
+        </is>
+      </c>
+      <c r="B162" s="2" t="inlineStr">
+        <is>
+          <t>Details of any voluntary agreements made as part of an oil and gas extraction application.</t>
+        </is>
+      </c>
       <c r="C162" s="2" t="inlineStr">
         <is>
-          <t>Agreement summary</t>
+          <t>Draft agreement included</t>
         </is>
       </c>
       <c r="D162" s="2" t="inlineStr"/>
@@ -5478,15 +5494,42 @@
       <c r="F162" s="2" t="inlineStr"/>
       <c r="G162" s="2" t="inlineStr">
         <is>
+          <t>Has an outline or draft agreement been included? (True / False)</t>
+        </is>
+      </c>
+      <c r="H162" s="2" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="I162" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n"/>
+      <c r="B163" s="2" t="n"/>
+      <c r="C163" s="2" t="inlineStr">
+        <is>
+          <t>Agreement summary</t>
+        </is>
+      </c>
+      <c r="D163" s="2" t="inlineStr"/>
+      <c r="E163" s="2" t="inlineStr"/>
+      <c r="F163" s="2" t="inlineStr"/>
+      <c r="G163" s="2" t="inlineStr">
+        <is>
           <t>Summary of the agreement</t>
         </is>
       </c>
-      <c r="H162" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I162" s="2" t="inlineStr">
+      <c r="H163" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I163" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -5494,7 +5537,6 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A151"/>
     <mergeCell ref="B149:B150"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="A57:A59"/>
@@ -5509,9 +5551,10 @@
     <mergeCell ref="B90:B97"/>
     <mergeCell ref="B124:B128"/>
     <mergeCell ref="A129:A137"/>
-    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="A162:A163"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="A84:A89"/>
+    <mergeCell ref="B151:B152"/>
     <mergeCell ref="A148"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A25:A32"/>
@@ -5525,29 +5568,29 @@
     <mergeCell ref="A90:A97"/>
     <mergeCell ref="A37:A42"/>
     <mergeCell ref="B121:B123"/>
+    <mergeCell ref="A151:A152"/>
     <mergeCell ref="B37:B42"/>
+    <mergeCell ref="B162:B163"/>
     <mergeCell ref="B56"/>
     <mergeCell ref="A79:A83"/>
-    <mergeCell ref="A152:A160"/>
     <mergeCell ref="B129:B137"/>
     <mergeCell ref="A113:A120"/>
     <mergeCell ref="B33:B36"/>
-    <mergeCell ref="B151"/>
     <mergeCell ref="B69:B78"/>
     <mergeCell ref="B60"/>
     <mergeCell ref="B84:B89"/>
     <mergeCell ref="B142:B147"/>
+    <mergeCell ref="B153:B161"/>
     <mergeCell ref="B148"/>
     <mergeCell ref="A61:A67"/>
     <mergeCell ref="A124:A128"/>
     <mergeCell ref="A56"/>
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="A2:A20"/>
-    <mergeCell ref="A161:A162"/>
     <mergeCell ref="B61:B67"/>
     <mergeCell ref="A43:A48"/>
+    <mergeCell ref="A153:A161"/>
     <mergeCell ref="B138:B141"/>
-    <mergeCell ref="B152:B160"/>
     <mergeCell ref="B113:B120"/>
     <mergeCell ref="A98:A112"/>
     <mergeCell ref="A142:A147"/>

</xml_diff>

<commit_message>
Latest generated outputs 2025-09-18
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/development-relating-to-the-onshore-extraction-of-oil-and-gas-extraction-oil-gas.xlsx
+++ b/generated/spreadsheet/development-relating-to-the-onshore-extraction-of-oil-and-gas-extraction-oil-gas.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I162"/>
+  <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5171,28 +5171,36 @@
           <t>Details of trees and/or hedges that will be affected by the proposed development</t>
         </is>
       </c>
-      <c r="C151" s="2" t="inlineStr"/>
+      <c r="C151" s="2" t="inlineStr">
+        <is>
+          <t>Trees on site</t>
+        </is>
+      </c>
       <c r="D151" s="2" t="inlineStr"/>
       <c r="E151" s="2" t="inlineStr"/>
       <c r="F151" s="2" t="inlineStr"/>
-      <c r="G151" s="2" t="inlineStr"/>
-      <c r="H151" s="2" t="inlineStr"/>
-      <c r="I151" s="2" t="inlineStr"/>
+      <c r="G151" s="2" t="inlineStr">
+        <is>
+          <t>Whether trees or hedges are present on the proposed development site</t>
+        </is>
+      </c>
+      <c r="H151" s="2" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="I151" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
     </row>
     <row r="152">
-      <c r="A152" s="2" t="inlineStr">
-        <is>
-          <t>Development type</t>
-        </is>
-      </c>
-      <c r="B152" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Supporting information for developments used for oil and gas exploration or mining </t>
-        </is>
-      </c>
+      <c r="A152" s="2" t="n"/>
+      <c r="B152" s="2" t="n"/>
       <c r="C152" s="2" t="inlineStr">
         <is>
-          <t>Development phase</t>
+          <t>Trees on adjacent land</t>
         </is>
       </c>
       <c r="D152" s="2" t="inlineStr"/>
@@ -5200,12 +5208,12 @@
       <c r="F152" s="2" t="inlineStr"/>
       <c r="G152" s="2" t="inlineStr">
         <is>
-          <t>Phases of oil and gas development the application covers</t>
+          <t>Whether trees or hedges on land adjacent to the proposed development site could influence the development or might be important as part of the local landscape character</t>
         </is>
       </c>
       <c r="H152" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I152" s="2" t="inlineStr">
@@ -5215,11 +5223,19 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="2" t="n"/>
-      <c r="B153" s="2" t="n"/>
+      <c r="A153" s="2" t="inlineStr">
+        <is>
+          <t>Development type</t>
+        </is>
+      </c>
+      <c r="B153" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Supporting information for developments used for oil and gas exploration or mining </t>
+        </is>
+      </c>
       <c r="C153" s="2" t="inlineStr">
         <is>
-          <t>Development description</t>
+          <t>Development phase</t>
         </is>
       </c>
       <c r="D153" s="2" t="inlineStr"/>
@@ -5227,12 +5243,12 @@
       <c r="F153" s="2" t="inlineStr"/>
       <c r="G153" s="2" t="inlineStr">
         <is>
-          <t>Brief description of the development, including main oils, gases, and machinery</t>
+          <t>Phases of oil and gas development the application covers</t>
         </is>
       </c>
       <c r="H153" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I153" s="2" t="inlineStr">
@@ -5246,7 +5262,7 @@
       <c r="B154" s="2" t="n"/>
       <c r="C154" s="2" t="inlineStr">
         <is>
-          <t>Quantity cubic metres</t>
+          <t>Development description</t>
         </is>
       </c>
       <c r="D154" s="2" t="inlineStr"/>
@@ -5254,12 +5270,12 @@
       <c r="F154" s="2" t="inlineStr"/>
       <c r="G154" s="2" t="inlineStr">
         <is>
-          <t>Quantity of oil or gas involved in cubic metres</t>
+          <t>Brief description of the development, including main oils, gases, and machinery</t>
         </is>
       </c>
       <c r="H154" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I154" s="2" t="inlineStr">
@@ -5273,7 +5289,7 @@
       <c r="B155" s="2" t="n"/>
       <c r="C155" s="2" t="inlineStr">
         <is>
-          <t>Permission period years</t>
+          <t>Quantity cubic metres</t>
         </is>
       </c>
       <c r="D155" s="2" t="inlineStr"/>
@@ -5281,7 +5297,7 @@
       <c r="F155" s="2" t="inlineStr"/>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Period of permission sought in years</t>
+          <t>Quantity of oil or gas involved in cubic metres</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
@@ -5291,7 +5307,7 @@
       </c>
       <c r="I155" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -5300,7 +5316,7 @@
       <c r="B156" s="2" t="n"/>
       <c r="C156" s="2" t="inlineStr">
         <is>
-          <t>Hydrocarbon licence block</t>
+          <t>Permission period years</t>
         </is>
       </c>
       <c r="D156" s="2" t="inlineStr"/>
@@ -5308,17 +5324,17 @@
       <c r="F156" s="2" t="inlineStr"/>
       <c r="G156" s="2" t="inlineStr">
         <is>
-          <t>Hydrocarbon licence block where the development is located</t>
+          <t>Period of permission sought in years</t>
         </is>
       </c>
       <c r="H156" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I156" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -5327,7 +5343,7 @@
       <c r="B157" s="2" t="n"/>
       <c r="C157" s="2" t="inlineStr">
         <is>
-          <t>Surface site area hectares</t>
+          <t>Hydrocarbon licence block</t>
         </is>
       </c>
       <c r="D157" s="2" t="inlineStr"/>
@@ -5335,17 +5351,17 @@
       <c r="F157" s="2" t="inlineStr"/>
       <c r="G157" s="2" t="inlineStr">
         <is>
-          <t>Surface site area in hectares</t>
+          <t>Hydrocarbon licence block where the development is located</t>
         </is>
       </c>
       <c r="H157" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I157" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -5354,7 +5370,7 @@
       <c r="B158" s="2" t="n"/>
       <c r="C158" s="2" t="inlineStr">
         <is>
-          <t>Site hectares provided by</t>
+          <t>Surface site area hectares</t>
         </is>
       </c>
       <c r="D158" s="2" t="inlineStr"/>
@@ -5362,12 +5378,12 @@
       <c r="F158" s="2" t="inlineStr"/>
       <c r="G158" s="2" t="inlineStr">
         <is>
-          <t>Who provided the site hectares value (applicant or system)</t>
+          <t>Surface site area in hectares</t>
         </is>
       </c>
       <c r="H158" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>number</t>
         </is>
       </c>
       <c r="I158" s="2" t="inlineStr">
@@ -5381,7 +5397,7 @@
       <c r="B159" s="2" t="n"/>
       <c r="C159" s="2" t="inlineStr">
         <is>
-          <t>Environmental statement</t>
+          <t>Site hectares provided by</t>
         </is>
       </c>
       <c r="D159" s="2" t="inlineStr"/>
@@ -5389,17 +5405,17 @@
       <c r="F159" s="2" t="inlineStr"/>
       <c r="G159" s="2" t="inlineStr">
         <is>
-          <t>Is an Environmental Statement attached to the application</t>
+          <t>Who provided the site hectares value (applicant or system)</t>
         </is>
       </c>
       <c r="H159" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I159" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -5408,7 +5424,7 @@
       <c r="B160" s="2" t="n"/>
       <c r="C160" s="2" t="inlineStr">
         <is>
-          <t>Environmental statement reference</t>
+          <t>Environmental statement</t>
         </is>
       </c>
       <c r="D160" s="2" t="inlineStr"/>
@@ -5416,34 +5432,26 @@
       <c r="F160" s="2" t="inlineStr"/>
       <c r="G160" s="2" t="inlineStr">
         <is>
-          <t>Reference to the environmental statement document</t>
+          <t>Is an Environmental Statement attached to the application</t>
         </is>
       </c>
       <c r="H160" s="2" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I160" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="2" t="inlineStr">
-        <is>
-          <t>Voluntary agreement</t>
-        </is>
-      </c>
-      <c r="B161" s="2" t="inlineStr">
-        <is>
-          <t>Details of any voluntary agreements made as part of an oil and gas extraction application.</t>
-        </is>
-      </c>
+      <c r="A161" s="2" t="n"/>
+      <c r="B161" s="2" t="n"/>
       <c r="C161" s="2" t="inlineStr">
         <is>
-          <t>Draft agreement included</t>
+          <t>Environmental statement reference</t>
         </is>
       </c>
       <c r="D161" s="2" t="inlineStr"/>
@@ -5451,26 +5459,34 @@
       <c r="F161" s="2" t="inlineStr"/>
       <c r="G161" s="2" t="inlineStr">
         <is>
-          <t>Has an outline or draft agreement been included? (True / False)</t>
+          <t>Reference to the environmental statement document</t>
         </is>
       </c>
       <c r="H161" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I161" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="2" t="n"/>
-      <c r="B162" s="2" t="n"/>
+      <c r="A162" s="2" t="inlineStr">
+        <is>
+          <t>Voluntary agreement</t>
+        </is>
+      </c>
+      <c r="B162" s="2" t="inlineStr">
+        <is>
+          <t>Details of any voluntary agreements made as part of an oil and gas extraction application.</t>
+        </is>
+      </c>
       <c r="C162" s="2" t="inlineStr">
         <is>
-          <t>Agreement summary</t>
+          <t>Draft agreement included</t>
         </is>
       </c>
       <c r="D162" s="2" t="inlineStr"/>
@@ -5478,15 +5494,42 @@
       <c r="F162" s="2" t="inlineStr"/>
       <c r="G162" s="2" t="inlineStr">
         <is>
+          <t>Has an outline or draft agreement been included? (True / False)</t>
+        </is>
+      </c>
+      <c r="H162" s="2" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="I162" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n"/>
+      <c r="B163" s="2" t="n"/>
+      <c r="C163" s="2" t="inlineStr">
+        <is>
+          <t>Agreement summary</t>
+        </is>
+      </c>
+      <c r="D163" s="2" t="inlineStr"/>
+      <c r="E163" s="2" t="inlineStr"/>
+      <c r="F163" s="2" t="inlineStr"/>
+      <c r="G163" s="2" t="inlineStr">
+        <is>
           <t>Summary of the agreement</t>
         </is>
       </c>
-      <c r="H162" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I162" s="2" t="inlineStr">
+      <c r="H163" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I163" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
@@ -5494,7 +5537,6 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A151"/>
     <mergeCell ref="B149:B150"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="A57:A59"/>
@@ -5509,9 +5551,10 @@
     <mergeCell ref="B90:B97"/>
     <mergeCell ref="B124:B128"/>
     <mergeCell ref="A129:A137"/>
-    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="A162:A163"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="A84:A89"/>
+    <mergeCell ref="B151:B152"/>
     <mergeCell ref="A148"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A25:A32"/>
@@ -5525,29 +5568,29 @@
     <mergeCell ref="A90:A97"/>
     <mergeCell ref="A37:A42"/>
     <mergeCell ref="B121:B123"/>
+    <mergeCell ref="A151:A152"/>
     <mergeCell ref="B37:B42"/>
+    <mergeCell ref="B162:B163"/>
     <mergeCell ref="B56"/>
     <mergeCell ref="A79:A83"/>
-    <mergeCell ref="A152:A160"/>
     <mergeCell ref="B129:B137"/>
     <mergeCell ref="A113:A120"/>
     <mergeCell ref="B33:B36"/>
-    <mergeCell ref="B151"/>
     <mergeCell ref="B69:B78"/>
     <mergeCell ref="B60"/>
     <mergeCell ref="B84:B89"/>
     <mergeCell ref="B142:B147"/>
+    <mergeCell ref="B153:B161"/>
     <mergeCell ref="B148"/>
     <mergeCell ref="A61:A67"/>
     <mergeCell ref="A124:A128"/>
     <mergeCell ref="A56"/>
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="A2:A20"/>
-    <mergeCell ref="A161:A162"/>
     <mergeCell ref="B61:B67"/>
     <mergeCell ref="A43:A48"/>
+    <mergeCell ref="A153:A161"/>
     <mergeCell ref="B138:B141"/>
-    <mergeCell ref="B152:B160"/>
     <mergeCell ref="B113:B120"/>
     <mergeCell ref="A98:A112"/>
     <mergeCell ref="A142:A147"/>

</xml_diff>

<commit_message>
Latest generated outputs 2025-09-24
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/development-relating-to-the-onshore-extraction-of-oil-and-gas-extraction-oil-gas.xlsx
+++ b/generated/spreadsheet/development-relating-to-the-onshore-extraction-of-oil-and-gas-extraction-oil-gas.xlsx
@@ -2394,7 +2394,7 @@
       </c>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>How the proposed development will impact employment, including existing and proposed employee numbers</t>
+          <t>How the proposed development will impact existing and proposed employee numbers</t>
         </is>
       </c>
       <c r="C61" s="2" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="B124" s="2" t="inlineStr">
         <is>
-          <t>Details of pre-application advice received from the planning authority</t>
+          <t>Details of pre-application advice previously received from the planning authority</t>
         </is>
       </c>
       <c r="C124" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Latest generated outputs 2025-12-05
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/development-relating-to-the-onshore-extraction-of-oil-and-gas-extraction-oil-gas.xlsx
+++ b/generated/spreadsheet/development-relating-to-the-onshore-extraction-of-oil-and-gas-extraction-oil-gas.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I174"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
     <col width="58" customWidth="1" min="1" max="1"/>
     <col width="72" customWidth="1" min="2" max="2"/>
     <col width="38" customWidth="1" min="3" max="3"/>
-    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="29" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
     <col width="72" customWidth="1" min="7" max="7"/>
@@ -5301,17 +5301,18 @@
     <row r="153">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>Development type</t>
+          <t>Oil and gas permission types</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Supporting information for developments used for oil and gas exploration or mining </t>
+          <t xml:space="preserve">Module for details about types of onshore oil and gas extraction permissions already received and applying for
+</t>
         </is>
       </c>
       <c r="C153" s="2" t="inlineStr">
         <is>
-          <t>Development phase</t>
+          <t>Oil and gas permission types[]</t>
         </is>
       </c>
       <c r="D153" s="2" t="inlineStr"/>
@@ -5319,7 +5320,7 @@
       <c r="F153" s="2" t="inlineStr"/>
       <c r="G153" s="2" t="inlineStr">
         <is>
-          <t>Phases of oil and gas development the application covers</t>
+          <t>List of permission types being applied for</t>
         </is>
       </c>
       <c r="H153" s="2" t="inlineStr">
@@ -5338,15 +5339,19 @@
       <c r="B154" s="2" t="n"/>
       <c r="C154" s="2" t="inlineStr">
         <is>
-          <t>Development description</t>
-        </is>
-      </c>
-      <c r="D154" s="2" t="inlineStr"/>
+          <t>Related permissions[]</t>
+        </is>
+      </c>
+      <c r="D154" s="2" t="inlineStr">
+        <is>
+          <t>Reference</t>
+        </is>
+      </c>
       <c r="E154" s="2" t="inlineStr"/>
       <c r="F154" s="2" t="inlineStr"/>
       <c r="G154" s="2" t="inlineStr">
         <is>
-          <t>Brief description of the development, including main oils, gases, and machinery</t>
+          <t>The reference for the related application that permission was received for</t>
         </is>
       </c>
       <c r="H154" s="2" t="inlineStr">
@@ -5365,20 +5370,24 @@
       <c r="B155" s="2" t="n"/>
       <c r="C155" s="2" t="inlineStr">
         <is>
-          <t>Quantity cubic metres</t>
-        </is>
-      </c>
-      <c r="D155" s="2" t="inlineStr"/>
+          <t>Related permissions[]</t>
+        </is>
+      </c>
+      <c r="D155" s="2" t="inlineStr">
+        <is>
+          <t>Oil and gas permission type</t>
+        </is>
+      </c>
       <c r="E155" s="2" t="inlineStr"/>
       <c r="F155" s="2" t="inlineStr"/>
       <c r="G155" s="2" t="inlineStr">
         <is>
-          <t>Quantity of oil or gas involved in cubic metres</t>
+          <t>An oil and gas related permission type</t>
         </is>
       </c>
       <c r="H155" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I155" s="2" t="inlineStr">
@@ -5392,25 +5401,29 @@
       <c r="B156" s="2" t="n"/>
       <c r="C156" s="2" t="inlineStr">
         <is>
-          <t>Permission period years</t>
-        </is>
-      </c>
-      <c r="D156" s="2" t="inlineStr"/>
+          <t>Related permissions[]</t>
+        </is>
+      </c>
+      <c r="D156" s="2" t="inlineStr">
+        <is>
+          <t>Decision date</t>
+        </is>
+      </c>
       <c r="E156" s="2" t="inlineStr"/>
       <c r="F156" s="2" t="inlineStr"/>
       <c r="G156" s="2" t="inlineStr">
         <is>
-          <t>Period of permission sought in years</t>
+          <t>The date when the decision was made, in YYYY-MM-DD format</t>
         </is>
       </c>
       <c r="H156" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I156" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -5419,15 +5432,19 @@
       <c r="B157" s="2" t="n"/>
       <c r="C157" s="2" t="inlineStr">
         <is>
-          <t>Hydrocarbon licence block</t>
-        </is>
-      </c>
-      <c r="D157" s="2" t="inlineStr"/>
+          <t>Related permissions[]</t>
+        </is>
+      </c>
+      <c r="D157" s="2" t="inlineStr">
+        <is>
+          <t>Condition number</t>
+        </is>
+      </c>
       <c r="E157" s="2" t="inlineStr"/>
       <c r="F157" s="2" t="inlineStr"/>
       <c r="G157" s="2" t="inlineStr">
         <is>
-          <t>Hydrocarbon licence block where the development is located</t>
+          <t>Number of any condition being breached</t>
         </is>
       </c>
       <c r="H157" s="2" t="inlineStr">
@@ -5437,7 +5454,7 @@
       </c>
       <c r="I157" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -5446,7 +5463,7 @@
       <c r="B158" s="2" t="n"/>
       <c r="C158" s="2" t="inlineStr">
         <is>
-          <t>Surface site area hectares</t>
+          <t>Other details</t>
         </is>
       </c>
       <c r="D158" s="2" t="inlineStr"/>
@@ -5454,12 +5471,12 @@
       <c r="F158" s="2" t="inlineStr"/>
       <c r="G158" s="2" t="inlineStr">
         <is>
-          <t>Surface site area in hectares</t>
+          <t>Explanation if other ground is selected</t>
         </is>
       </c>
       <c r="H158" s="2" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I158" s="2" t="inlineStr">
@@ -5473,7 +5490,7 @@
       <c r="B159" s="2" t="n"/>
       <c r="C159" s="2" t="inlineStr">
         <is>
-          <t>Site hectares provided by</t>
+          <t>Will consolidate permissions</t>
         </is>
       </c>
       <c r="D159" s="2" t="inlineStr"/>
@@ -5481,17 +5498,17 @@
       <c r="F159" s="2" t="inlineStr"/>
       <c r="G159" s="2" t="inlineStr">
         <is>
-          <t>Who provided the site hectares value (applicant or system)</t>
+          <t>Is the applicant looking to consolidate permissions?</t>
         </is>
       </c>
       <c r="H159" s="2" t="inlineStr">
         <is>
-          <t>enum</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="I159" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
@@ -5500,7 +5517,7 @@
       <c r="B160" s="2" t="n"/>
       <c r="C160" s="2" t="inlineStr">
         <is>
-          <t>Environmental statement</t>
+          <t>Details</t>
         </is>
       </c>
       <c r="D160" s="2" t="inlineStr"/>
@@ -5508,17 +5525,17 @@
       <c r="F160" s="2" t="inlineStr"/>
       <c r="G160" s="2" t="inlineStr">
         <is>
-          <t>Is an Environmental Statement attached to the application</t>
+          <t>Details about the consolidation or update of permissions</t>
         </is>
       </c>
       <c r="H160" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>string</t>
         </is>
       </c>
       <c r="I160" s="2" t="inlineStr">
         <is>
-          <t>MUST</t>
+          <t>MAY</t>
         </is>
       </c>
     </row>
@@ -5527,15 +5544,19 @@
       <c r="B161" s="2" t="n"/>
       <c r="C161" s="2" t="inlineStr">
         <is>
-          <t>Environmental statement reference</t>
-        </is>
-      </c>
-      <c r="D161" s="2" t="inlineStr"/>
+          <t>Related proposals[]</t>
+        </is>
+      </c>
+      <c r="D161" s="2" t="inlineStr">
+        <is>
+          <t>Reference</t>
+        </is>
+      </c>
       <c r="E161" s="2" t="inlineStr"/>
       <c r="F161" s="2" t="inlineStr"/>
       <c r="G161" s="2" t="inlineStr">
         <is>
-          <t>Reference to the environmental statement document</t>
+          <t>The reference for the related application</t>
         </is>
       </c>
       <c r="H161" s="2" t="inlineStr">
@@ -5545,37 +5566,33 @@
       </c>
       <c r="I161" s="2" t="inlineStr">
         <is>
-          <t>MAY</t>
+          <t>MUST</t>
         </is>
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="2" t="inlineStr">
-        <is>
-          <t>Voluntary agreement</t>
-        </is>
-      </c>
-      <c r="B162" s="2" t="inlineStr">
-        <is>
-          <t>Details of any voluntary agreements made as part of an oil and gas extraction application.</t>
-        </is>
-      </c>
+      <c r="A162" s="2" t="n"/>
+      <c r="B162" s="2" t="n"/>
       <c r="C162" s="2" t="inlineStr">
         <is>
-          <t>Draft agreement included</t>
-        </is>
-      </c>
-      <c r="D162" s="2" t="inlineStr"/>
+          <t>Related proposals[]</t>
+        </is>
+      </c>
+      <c r="D162" s="2" t="inlineStr">
+        <is>
+          <t>Application type</t>
+        </is>
+      </c>
       <c r="E162" s="2" t="inlineStr"/>
       <c r="F162" s="2" t="inlineStr"/>
       <c r="G162" s="2" t="inlineStr">
         <is>
-          <t>Has an outline or draft agreement been included? (True / False)</t>
+          <t>The type of planning application</t>
         </is>
       </c>
       <c r="H162" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I162" s="2" t="inlineStr">
@@ -5589,30 +5606,347 @@
       <c r="B163" s="2" t="n"/>
       <c r="C163" s="2" t="inlineStr">
         <is>
-          <t>Agreement summary</t>
-        </is>
-      </c>
-      <c r="D163" s="2" t="inlineStr"/>
+          <t>Related proposals[]</t>
+        </is>
+      </c>
+      <c r="D163" s="2" t="inlineStr">
+        <is>
+          <t>Decision date</t>
+        </is>
+      </c>
       <c r="E163" s="2" t="inlineStr"/>
       <c r="F163" s="2" t="inlineStr"/>
       <c r="G163" s="2" t="inlineStr">
         <is>
+          <t>The date when the decision was made, in YYYY-MM-DD format</t>
+        </is>
+      </c>
+      <c r="H163" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I163" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="inlineStr">
+        <is>
+          <t>Development type</t>
+        </is>
+      </c>
+      <c r="B164" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Supporting information for developments used for oil and gas exploration or mining </t>
+        </is>
+      </c>
+      <c r="C164" s="2" t="inlineStr">
+        <is>
+          <t>Development phase</t>
+        </is>
+      </c>
+      <c r="D164" s="2" t="inlineStr"/>
+      <c r="E164" s="2" t="inlineStr"/>
+      <c r="F164" s="2" t="inlineStr"/>
+      <c r="G164" s="2" t="inlineStr">
+        <is>
+          <t>Phases of oil and gas development the application covers</t>
+        </is>
+      </c>
+      <c r="H164" s="2" t="inlineStr">
+        <is>
+          <t>enum</t>
+        </is>
+      </c>
+      <c r="I164" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="n"/>
+      <c r="B165" s="2" t="n"/>
+      <c r="C165" s="2" t="inlineStr">
+        <is>
+          <t>Development description</t>
+        </is>
+      </c>
+      <c r="D165" s="2" t="inlineStr"/>
+      <c r="E165" s="2" t="inlineStr"/>
+      <c r="F165" s="2" t="inlineStr"/>
+      <c r="G165" s="2" t="inlineStr">
+        <is>
+          <t>Brief description of the development, including main oils, gases, and machinery</t>
+        </is>
+      </c>
+      <c r="H165" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I165" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n"/>
+      <c r="B166" s="2" t="n"/>
+      <c r="C166" s="2" t="inlineStr">
+        <is>
+          <t>Quantity cubic metres</t>
+        </is>
+      </c>
+      <c r="D166" s="2" t="inlineStr"/>
+      <c r="E166" s="2" t="inlineStr"/>
+      <c r="F166" s="2" t="inlineStr"/>
+      <c r="G166" s="2" t="inlineStr">
+        <is>
+          <t>Quantity of oil or gas involved in cubic metres</t>
+        </is>
+      </c>
+      <c r="H166" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="I166" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n"/>
+      <c r="B167" s="2" t="n"/>
+      <c r="C167" s="2" t="inlineStr">
+        <is>
+          <t>Permission period years</t>
+        </is>
+      </c>
+      <c r="D167" s="2" t="inlineStr"/>
+      <c r="E167" s="2" t="inlineStr"/>
+      <c r="F167" s="2" t="inlineStr"/>
+      <c r="G167" s="2" t="inlineStr">
+        <is>
+          <t>Period of permission sought in years</t>
+        </is>
+      </c>
+      <c r="H167" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="I167" s="2" t="inlineStr">
+        <is>
+          <t>MAY</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="n"/>
+      <c r="B168" s="2" t="n"/>
+      <c r="C168" s="2" t="inlineStr">
+        <is>
+          <t>Hydrocarbon licence block</t>
+        </is>
+      </c>
+      <c r="D168" s="2" t="inlineStr"/>
+      <c r="E168" s="2" t="inlineStr"/>
+      <c r="F168" s="2" t="inlineStr"/>
+      <c r="G168" s="2" t="inlineStr">
+        <is>
+          <t>Hydrocarbon licence block where the development is located</t>
+        </is>
+      </c>
+      <c r="H168" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I168" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n"/>
+      <c r="B169" s="2" t="n"/>
+      <c r="C169" s="2" t="inlineStr">
+        <is>
+          <t>Surface site area hectares</t>
+        </is>
+      </c>
+      <c r="D169" s="2" t="inlineStr"/>
+      <c r="E169" s="2" t="inlineStr"/>
+      <c r="F169" s="2" t="inlineStr"/>
+      <c r="G169" s="2" t="inlineStr">
+        <is>
+          <t>Surface site area in hectares</t>
+        </is>
+      </c>
+      <c r="H169" s="2" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="I169" s="2" t="inlineStr">
+        <is>
+          <t>MAY</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n"/>
+      <c r="B170" s="2" t="n"/>
+      <c r="C170" s="2" t="inlineStr">
+        <is>
+          <t>Site hectares provided by</t>
+        </is>
+      </c>
+      <c r="D170" s="2" t="inlineStr"/>
+      <c r="E170" s="2" t="inlineStr"/>
+      <c r="F170" s="2" t="inlineStr"/>
+      <c r="G170" s="2" t="inlineStr">
+        <is>
+          <t>Who provided the site hectares value (applicant or system)</t>
+        </is>
+      </c>
+      <c r="H170" s="2" t="inlineStr">
+        <is>
+          <t>enum</t>
+        </is>
+      </c>
+      <c r="I170" s="2" t="inlineStr">
+        <is>
+          <t>MAY</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="n"/>
+      <c r="B171" s="2" t="n"/>
+      <c r="C171" s="2" t="inlineStr">
+        <is>
+          <t>Environmental statement</t>
+        </is>
+      </c>
+      <c r="D171" s="2" t="inlineStr"/>
+      <c r="E171" s="2" t="inlineStr"/>
+      <c r="F171" s="2" t="inlineStr"/>
+      <c r="G171" s="2" t="inlineStr">
+        <is>
+          <t>Is an Environmental Statement attached to the application</t>
+        </is>
+      </c>
+      <c r="H171" s="2" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="I171" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="n"/>
+      <c r="B172" s="2" t="n"/>
+      <c r="C172" s="2" t="inlineStr">
+        <is>
+          <t>Environmental statement reference</t>
+        </is>
+      </c>
+      <c r="D172" s="2" t="inlineStr"/>
+      <c r="E172" s="2" t="inlineStr"/>
+      <c r="F172" s="2" t="inlineStr"/>
+      <c r="G172" s="2" t="inlineStr">
+        <is>
+          <t>Reference to the environmental statement document</t>
+        </is>
+      </c>
+      <c r="H172" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I172" s="2" t="inlineStr">
+        <is>
+          <t>MAY</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="2" t="inlineStr">
+        <is>
+          <t>Voluntary agreement</t>
+        </is>
+      </c>
+      <c r="B173" s="2" t="inlineStr">
+        <is>
+          <t>Details of any voluntary agreements made as part of an oil and gas extraction application.</t>
+        </is>
+      </c>
+      <c r="C173" s="2" t="inlineStr">
+        <is>
+          <t>Draft agreement included</t>
+        </is>
+      </c>
+      <c r="D173" s="2" t="inlineStr"/>
+      <c r="E173" s="2" t="inlineStr"/>
+      <c r="F173" s="2" t="inlineStr"/>
+      <c r="G173" s="2" t="inlineStr">
+        <is>
+          <t>Has an outline or draft agreement been included? (True / False)</t>
+        </is>
+      </c>
+      <c r="H173" s="2" t="inlineStr">
+        <is>
+          <t>boolean</t>
+        </is>
+      </c>
+      <c r="I173" s="2" t="inlineStr">
+        <is>
+          <t>MUST</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="n"/>
+      <c r="B174" s="2" t="n"/>
+      <c r="C174" s="2" t="inlineStr">
+        <is>
+          <t>Agreement summary</t>
+        </is>
+      </c>
+      <c r="D174" s="2" t="inlineStr"/>
+      <c r="E174" s="2" t="inlineStr"/>
+      <c r="F174" s="2" t="inlineStr"/>
+      <c r="G174" s="2" t="inlineStr">
+        <is>
           <t>Summary of the agreement</t>
         </is>
       </c>
-      <c r="H163" s="2" t="inlineStr">
-        <is>
-          <t>string</t>
-        </is>
-      </c>
-      <c r="I163" s="2" t="inlineStr">
+      <c r="H174" s="2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="I174" s="2" t="inlineStr">
         <is>
           <t>MAY</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="58">
+  <mergeCells count="60">
     <mergeCell ref="B149:B150"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="A57:A59"/>
@@ -5622,12 +5956,12 @@
     <mergeCell ref="B25:B32"/>
     <mergeCell ref="B43:B48"/>
     <mergeCell ref="A138:A141"/>
+    <mergeCell ref="A164:A172"/>
     <mergeCell ref="A68"/>
     <mergeCell ref="A121:A123"/>
     <mergeCell ref="B90:B97"/>
     <mergeCell ref="B124:B128"/>
     <mergeCell ref="A129:A137"/>
-    <mergeCell ref="A162:A163"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="A84:A89"/>
     <mergeCell ref="B151:B152"/>
@@ -5646,28 +5980,30 @@
     <mergeCell ref="B121:B123"/>
     <mergeCell ref="A151:A152"/>
     <mergeCell ref="B37:B42"/>
-    <mergeCell ref="B162:B163"/>
     <mergeCell ref="B56"/>
+    <mergeCell ref="B164:B172"/>
     <mergeCell ref="A79:A83"/>
     <mergeCell ref="B129:B137"/>
     <mergeCell ref="A113:A120"/>
     <mergeCell ref="B33:B36"/>
+    <mergeCell ref="B173:B174"/>
     <mergeCell ref="B69:B78"/>
     <mergeCell ref="B60"/>
     <mergeCell ref="B84:B89"/>
     <mergeCell ref="B142:B147"/>
-    <mergeCell ref="B153:B161"/>
     <mergeCell ref="B148"/>
     <mergeCell ref="A61:A67"/>
     <mergeCell ref="A124:A128"/>
     <mergeCell ref="A56"/>
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="A2:A20"/>
+    <mergeCell ref="B153:B163"/>
     <mergeCell ref="B61:B67"/>
     <mergeCell ref="A43:A48"/>
-    <mergeCell ref="A153:A161"/>
     <mergeCell ref="B138:B141"/>
+    <mergeCell ref="A153:A163"/>
     <mergeCell ref="B113:B120"/>
+    <mergeCell ref="A173:A174"/>
     <mergeCell ref="A98:A112"/>
     <mergeCell ref="A142:A147"/>
     <mergeCell ref="A52:A55"/>

</xml_diff>

<commit_message>
Latest generated outputs 2026-01-15
</commit_message>
<xml_diff>
--- a/generated/spreadsheet/development-relating-to-the-onshore-extraction-of-oil-and-gas-extraction-oil-gas.xlsx
+++ b/generated/spreadsheet/development-relating-to-the-onshore-extraction-of-oil-and-gas-extraction-oil-gas.xlsx
@@ -437,7 +437,7 @@
   <cols>
     <col width="58" customWidth="1" min="1" max="1"/>
     <col width="72" customWidth="1" min="2" max="2"/>
-    <col width="38" customWidth="1" min="3" max="3"/>
+    <col width="42" customWidth="1" min="3" max="3"/>
     <col width="29" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
@@ -3032,7 +3032,7 @@
       <c r="B80" s="2" t="n"/>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>Connect to drainage system</t>
+          <t>Connect to drainage system (oil and gas)</t>
         </is>
       </c>
       <c r="D80" s="2" t="inlineStr"/>
@@ -3040,12 +3040,12 @@
       <c r="F80" s="2" t="inlineStr"/>
       <c r="G80" s="2" t="inlineStr">
         <is>
-          <t>Whether the proposal needs to connect to the existing drainage system</t>
+          <t>Whether the proposal needs to connect to the existing drainage system (oil and gas applications)</t>
         </is>
       </c>
       <c r="H80" s="2" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>enum</t>
         </is>
       </c>
       <c r="I80" s="2" t="inlineStr">

</xml_diff>